<commit_message>
make a class for data parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-measuring.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-measuring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
@@ -91,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +119,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -152,6 +158,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,33 +508,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="7"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="7"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="7"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="7"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="7"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
@@ -870,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
convert more parsers to use classes
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-measuring.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-measuring.xlsx
@@ -444,7 +444,7 @@
   <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>